<commit_message>
Advance in the .xslx
</commit_message>
<xml_diff>
--- a/Vacaciones.xlsx
+++ b/Vacaciones.xlsx
@@ -3,10 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Recursos Humanos" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Departamento 1 " sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Departamento 2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr/>
   <extLst>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -24,7 +25,22 @@
     <t xml:space="preserve">Departamento :</t>
   </si>
   <si>
-    <t xml:space="preserve">Recursos Humanos </t>
+    <t xml:space="preserve">Nombre </t>
+  </si>
+  <si>
+    <t>ID(Matricula)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Días de vacaciones </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estado </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fecha de ingreso </t>
+  </si>
+  <si>
+    <t>´</t>
   </si>
 </sst>
 </file>
@@ -59,11 +75,12 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,6 +584,11 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="13.00390625"/>
+    <col customWidth="1" min="3" max="3" width="18.421875"/>
+    <col customWidth="1" min="5" max="5" width="17.421875"/>
+  </cols>
   <sheetData>
     <row r="1" ht="14.25">
       <c r="A1" t="s">
@@ -578,10 +600,101 @@
         <v>1</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="D7" s="1"/>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="I10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+  </mergeCells>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="13.00390625"/>
+    <col customWidth="1" min="3" max="3" width="18.421875"/>
+    <col customWidth="1" min="5" max="5" width="17.421875"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1">
+        <v>2</v>
+      </c>
       <c r="E2" s="1"/>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="D7" s="1"/>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="I10" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>